<commit_message>
updates to vaccines info
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{D79920B0-6205-4074-8049-208E28762C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1FCC3819-13A4-4752-8B03-ED2AF6D48F54}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{D79920B0-6205-4074-8049-208E28762C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BADB9501-9031-4A83-81E4-D94586420B14}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5172" windowWidth="30612" windowHeight="11508" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="0" yWindow="5604" windowWidth="30612" windowHeight="11076" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>manufacturer</t>
   </si>
@@ -66,12 +66,6 @@
     <t>type info</t>
   </si>
   <si>
-    <t>supply chain</t>
-  </si>
-  <si>
-    <t>(link)</t>
-  </si>
-  <si>
     <t>reserved doses</t>
   </si>
   <si>
@@ -183,12 +177,6 @@
     <t>vaccination plan</t>
   </si>
   <si>
-    <t>3 weeks gab between shots</t>
-  </si>
-  <si>
-    <t>4 weeks gab between doses</t>
-  </si>
-  <si>
     <t>4-12 week gap / TBD</t>
   </si>
   <si>
@@ -250,6 +238,15 @@
   </si>
   <si>
     <t>nature comment:</t>
+  </si>
+  <si>
+    <t>cooling temperature</t>
+  </si>
+  <si>
+    <t>4 weeks gap between doses</t>
+  </si>
+  <si>
+    <t>3 weeks gap between shots</t>
   </si>
 </sst>
 </file>
@@ -658,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -681,16 +678,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -702,25 +699,25 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -728,19 +725,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2">
         <v>0.95</v>
@@ -749,13 +746,13 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="L2" t="s">
         <v>7</v>
@@ -775,19 +772,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2">
         <v>0.94</v>
@@ -796,13 +793,13 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
@@ -822,40 +819,38 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>39</v>
       </c>
       <c r="N4" s="5">
         <v>5300000</v>
@@ -866,47 +861,43 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
         <v>37</v>
       </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -927,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -940,32 +931,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -973,46 +964,46 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1202,18 +1193,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1235,18 +1226,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corrections for step function
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="214" documentId="8_{D79920B0-6205-4074-8049-208E28762C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B8B7D41-DD9C-40DD-89FD-E969DB287EBC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5604" windowWidth="30612" windowHeight="11076" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="0" yWindow="3636" windowWidth="30612" windowHeight="9432" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -659,7 +659,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1198,18 +1198,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1231,18 +1231,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added translation for vaccine info
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{D79920B0-6205-4074-8049-208E28762C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B8B7D41-DD9C-40DD-89FD-E969DB287EBC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905FC65A-DBD8-4EB9-864B-D24DCDA24B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3636" windowWidth="30612" windowHeight="9432" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>manufacturer</t>
   </si>
@@ -96,12 +96,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>information about vaccines, information about agreements with vaccine producers</t>
-  </si>
-  <si>
     <t>agreement date</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>approved for age</t>
   </si>
   <si>
-    <t>short summary of the vaccines</t>
-  </si>
-  <si>
     <t>COVID-19 Vaccine Moderna</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Next-generation vaccine platforms for COVID-19</t>
   </si>
   <si>
-    <t>BAG:</t>
-  </si>
-  <si>
     <t>SRF:</t>
   </si>
   <si>
@@ -250,6 +238,39 @@
   </si>
   <si>
     <t>COVID-19 Vaccine AstraZeneca</t>
+  </si>
+  <si>
+    <t>Bundesamt für Statistik (BAG)</t>
+  </si>
+  <si>
+    <t>details_en</t>
+  </si>
+  <si>
+    <t>details_de</t>
+  </si>
+  <si>
+    <t>information about vaccines and agreements with vaccine producers</t>
+  </si>
+  <si>
+    <t>Information zu den Impfstoffen und Verträgen mit Herstellern</t>
+  </si>
+  <si>
+    <t>Informationen zu den Impfstoffen</t>
+  </si>
+  <si>
+    <t>information about the vaccines</t>
+  </si>
+  <si>
+    <t>press release: Janssen-Cilag AG reicht Zulassungsgesuch für ihren Impfstoffkandidaten ein</t>
+  </si>
+  <si>
+    <t>wie und warum Impfstoffe im Körper wirken</t>
+  </si>
+  <si>
+    <t>How vaccine technology, choice and supply work in Switzerland (english)</t>
+  </si>
+  <si>
+    <t>Next-generation vaccine platforms for COVID-19 (english)</t>
   </si>
 </sst>
 </file>
@@ -658,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -681,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -702,13 +723,13 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -720,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -731,13 +752,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>14</v>
@@ -749,13 +770,13 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
         <v>7</v>
@@ -775,16 +796,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>14</v>
@@ -796,13 +817,13 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
@@ -822,38 +843,38 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
       </c>
       <c r="N4" s="5">
         <v>5300000</v>
@@ -867,38 +888,38 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>
       <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" t="s">
-        <v>37</v>
-      </c>
       <c r="L5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N5" s="5">
         <v>0</v>
@@ -921,99 +942,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="117.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.21875" customWidth="1"/>
+    <col min="4" max="4" width="117.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1198,18 +1241,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1231,18 +1274,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated number of reserved doses, new vaccines
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905FC65A-DBD8-4EB9-864B-D24DCDA24B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E18D6D3-FD32-4D1E-8C8E-0F850ED3771C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="30720" windowHeight="10116" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
   <si>
     <t>manufacturer</t>
   </si>
@@ -271,6 +271,48 @@
   </si>
   <si>
     <t>Next-generation vaccine platforms for COVID-19 (english)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wikipedia: </t>
+  </si>
+  <si>
+    <t>COVID-19 vaccine</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2-Impfstoff</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/SARS-CoV-2-Impfstoff</t>
+  </si>
+  <si>
+    <t>Curevac</t>
+  </si>
+  <si>
+    <t>Zorecimeran</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/CVnCoV</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>not approved</t>
+  </si>
+  <si>
+    <t>Novavax</t>
+  </si>
+  <si>
+    <t>NVX-CoV2373</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Novavax_COVID-19_vaccine</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>recombinant nanoparticle vaccine</t>
   </si>
 </sst>
 </file>
@@ -679,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -832,7 +874,7 @@
         <v>44208</v>
       </c>
       <c r="N3" s="5">
-        <v>7500000</v>
+        <v>13500000</v>
       </c>
       <c r="O3" s="8">
         <v>44050</v>
@@ -927,25 +969,111 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="5">
+        <v>5000000</v>
+      </c>
+      <c r="O6" s="8">
+        <v>44230</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="5">
+        <v>6000000</v>
+      </c>
+      <c r="O7" s="8">
+        <v>44230</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{AA5AA6B6-ABB5-48C2-9260-9D4AA70505D2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1054,15 +1182,36 @@
         <v>56</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{C67C19B8-C4B8-4EC7-9BB4-19ED833F6A9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -1240,12 +1389,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1256,6 +1399,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1273,15 +1425,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added i18 support in data_vaccines_information
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9787B916-3E82-4828-BDCF-FF4D45A0F365}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="-7284" yWindow="2040" windowWidth="14904" windowHeight="8496" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>manufacturer</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Informationen zu den Impfstoffen</t>
   </si>
   <si>
-    <t>information about the vaccines</t>
-  </si>
-  <si>
     <t>press release: Janssen-Cilag AG reicht Zulassungsgesuch für ihren Impfstoffkandidaten ein</t>
   </si>
   <si>
@@ -301,6 +298,60 @@
   </si>
   <si>
     <t>4-12 week gap</t>
+  </si>
+  <si>
+    <t>details_fr</t>
+  </si>
+  <si>
+    <t>informations sur les vaccins et les accords avec les producteurs de vaccins</t>
+  </si>
+  <si>
+    <t>comment et pourquoi les vaccins agissent dans l'organisme.</t>
+  </si>
+  <si>
+    <t>Vaccin contre la Covid-19</t>
+  </si>
+  <si>
+    <t>link_de</t>
+  </si>
+  <si>
+    <t>link_en</t>
+  </si>
+  <si>
+    <t>link_fr</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Vaccin_contre_la_Covid-19</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/COVID-19_vaccine</t>
+  </si>
+  <si>
+    <t>https://www.swissmedic.ch/swissmedic/de/home/ueber-uns/publikationen/video/way-vaccination-works.html</t>
+  </si>
+  <si>
+    <t>https://www.swissmedic.ch/swissmedic/fr/home/notre-profil/publications/video/way-vaccination-works.html</t>
+  </si>
+  <si>
+    <t>https://www.admin.ch/gov/de/start/dokumentation/medienmitteilungen.msg-id-81505.html</t>
+  </si>
+  <si>
+    <t>communiqué de presse : Janssen-Cilag SA soumet une demande d’autorisation pour son candidat vaccin</t>
+  </si>
+  <si>
+    <t>https://www.admin.ch/gov/fr/accueil/documentation/communiques.msg-id-81505.html</t>
+  </si>
+  <si>
+    <t>informations sur les vaccins (allemand)</t>
+  </si>
+  <si>
+    <t>information about the vaccines (german)</t>
+  </si>
+  <si>
+    <t>https://www.bag.admin.ch/bag/de/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/impfen.html</t>
+  </si>
+  <si>
+    <t>https://www.bag.admin.ch/bag/fr/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/impfen.html</t>
   </si>
 </sst>
 </file>
@@ -709,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -892,10 +943,10 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" t="s">
         <v>40</v>
@@ -904,7 +955,7 @@
         <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N4" s="5">
         <v>5300000</v>
@@ -931,7 +982,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -940,7 +991,7 @@
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
@@ -949,7 +1000,7 @@
         <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N5" s="5">
         <v>0</v>
@@ -958,16 +1009,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
         <v>78</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" t="s">
         <v>80</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -976,7 +1027,7 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -985,7 +1036,7 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
@@ -994,7 +1045,7 @@
         <v>32</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N6" s="5">
         <v>5000000</v>
@@ -1005,22 +1056,22 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>84</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>85</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>86</v>
       </c>
-      <c r="E7" t="s">
-        <v>87</v>
-      </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1029,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
         <v>40</v>
@@ -1038,7 +1089,7 @@
         <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N7" s="5">
         <v>6000000</v>
@@ -1058,21 +1109,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.21875" customWidth="1"/>
-    <col min="4" max="4" width="117.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="68.21875" customWidth="1"/>
+    <col min="5" max="5" width="117.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1083,10 +1134,22 @@
         <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1096,25 +1159,49 @@
       <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
       <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1122,13 +1209,25 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
         <v>34</v>
       </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1136,13 +1235,25 @@
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1150,13 +1261,25 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1164,32 +1287,59 @@
         <v>52</v>
       </c>
       <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>74</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>77</v>
+      <c r="F8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{C67C19B8-C4B8-4EC7-9BB4-19ED833F6A9E}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{C67C19B8-C4B8-4EC7-9BB4-19ED833F6A9E}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{DE30262E-6002-4DA8-B4D5-4CDF00B10510}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{382C03B7-1942-4F53-8F24-A40AC7CC5598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1200,15 +1350,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -1386,6 +1527,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
@@ -1396,14 +1546,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1419,4 +1561,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
i18n vaccines_information for list
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9787B916-3E82-4828-BDCF-FF4D45A0F365}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6000A9F2-BF7D-4841-B001-EF750617AAD3}"/>
   <bookViews>
-    <workbookView xWindow="-7284" yWindow="2040" windowWidth="14904" windowHeight="8496" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="163">
   <si>
     <t>manufacturer</t>
   </si>
@@ -352,6 +352,177 @@
   </si>
   <si>
     <t>https://www.bag.admin.ch/bag/fr/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/impfen.html</t>
+  </si>
+  <si>
+    <t>vaccine type_en</t>
+  </si>
+  <si>
+    <t>vaccine type_de</t>
+  </si>
+  <si>
+    <t>vaccine type_fr</t>
+  </si>
+  <si>
+    <t>mRNA Impfstoff</t>
+  </si>
+  <si>
+    <t>Viraler-Vektor-Impfstoff, basierend auf Adenovirus aus Schimpansen</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/AZD1222</t>
+  </si>
+  <si>
+    <t>Viraler-Vektor-Impfstoff, basierend auf menschlichen Adenovirus</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/AZD1222</t>
+  </si>
+  <si>
+    <t>vaccine wikipedia_en</t>
+  </si>
+  <si>
+    <t>vaccine wikipedia_de</t>
+  </si>
+  <si>
+    <t>vaccine wikipedia_fr</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/NVX-CoV2373</t>
+  </si>
+  <si>
+    <t>rekombinanten Nanopartikel-Impfstoff</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/NVX-CoV2373</t>
+  </si>
+  <si>
+    <t>vaccin à nanoparticules recombinantes</t>
+  </si>
+  <si>
+    <t>mRNA vaccin</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Ad26.COV2.S</t>
+  </si>
+  <si>
+    <t>vaccin à vecteur viral, basé sur l'adénovirus humain</t>
+  </si>
+  <si>
+    <t>vaccin à vecteur viral, basé sur l'adénovirus des chimpanzés</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Ad26.COV2.S</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/MRNA-1273</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/MRNA-1273</t>
+  </si>
+  <si>
+    <t>vaccination plan_en</t>
+  </si>
+  <si>
+    <t>vaccination plan_fr</t>
+  </si>
+  <si>
+    <t>vaccination plan_de</t>
+  </si>
+  <si>
+    <t>3 Wochen zwischen 1. und 2. Impfdosis</t>
+  </si>
+  <si>
+    <t>4 Wochen zwischen 1. und 2. Impfdosis</t>
+  </si>
+  <si>
+    <t>4-12 Wochen zwischen 1. und 2. Impfdosis</t>
+  </si>
+  <si>
+    <t>3 semaines entre la 1ère et la 2ème dose de vaccin</t>
+  </si>
+  <si>
+    <t>4 semaines entre la 1ère et la 2ème dose de vaccin</t>
+  </si>
+  <si>
+    <t>4-12 semaines entre la 1ère et la 2ème dose de vaccin</t>
+  </si>
+  <si>
+    <t>approved for age_en</t>
+  </si>
+  <si>
+    <t>approved for age_de</t>
+  </si>
+  <si>
+    <t>approved for age_fr</t>
+  </si>
+  <si>
+    <t>16 und älter</t>
+  </si>
+  <si>
+    <t>18 und älter</t>
+  </si>
+  <si>
+    <t>nicht zugelassen</t>
+  </si>
+  <si>
+    <t>16 ans et plus</t>
+  </si>
+  <si>
+    <t>18 ans et plus</t>
+  </si>
+  <si>
+    <t>non autorisé</t>
+  </si>
+  <si>
+    <t>cooling temperature_en</t>
+  </si>
+  <si>
+    <t>cooling temperature_de</t>
+  </si>
+  <si>
+    <t>cooling temperature_fr</t>
+  </si>
+  <si>
+    <t>normale Kühlschranktemperatur</t>
+  </si>
+  <si>
+    <t>température normale du réfrigérateur</t>
+  </si>
+  <si>
+    <t>non connu</t>
+  </si>
+  <si>
+    <t>nicht bekannt</t>
+  </si>
+  <si>
+    <t>status_en</t>
+  </si>
+  <si>
+    <t>status_de</t>
+  </si>
+  <si>
+    <t>status_fr</t>
+  </si>
+  <si>
+    <t>zugelassen</t>
+  </si>
+  <si>
+    <t>im Zulassungsverfahren</t>
+  </si>
+  <si>
+    <t>en cours de procédure d'approbation</t>
+  </si>
+  <si>
+    <t>autorisé</t>
+  </si>
+  <si>
+    <t>effectiveness_en</t>
+  </si>
+  <si>
+    <t>effectiveness_de</t>
+  </si>
+  <si>
+    <t>effectiveness_fr</t>
   </si>
 </sst>
 </file>
@@ -758,27 +929,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.44140625" customWidth="1"/>
+    <col min="3" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="47.21875" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="29" width="14.77734375" customWidth="1"/>
+    <col min="30" max="30" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="8.44140625" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,43 +962,106 @@
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AE1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -835,44 +1071,101 @@
       <c r="C2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2">
+      <c r="M2" s="2">
         <v>0.95</v>
       </c>
-      <c r="H2">
+      <c r="N2" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="Q2">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="R2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" t="s">
+      <c r="S2" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" t="s">
+        <v>134</v>
+      </c>
+      <c r="V2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L2" t="s">
+      <c r="AA2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="9"/>
+      <c r="AD2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="6">
+      <c r="AE2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="6">
         <v>44184</v>
       </c>
-      <c r="N2" s="5">
+      <c r="AI2" s="5">
         <v>3000000</v>
       </c>
-      <c r="O2" s="8">
+      <c r="AJ2" s="8">
         <v>44172</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -882,89 +1175,213 @@
       <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2">
+      <c r="M3" s="2">
         <v>0.94</v>
       </c>
-      <c r="H3">
+      <c r="N3" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="R3" t="s">
         <v>60</v>
       </c>
-      <c r="J3" t="s">
+      <c r="S3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="W3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="AA3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC3" s="10"/>
+      <c r="AD3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6">
+      <c r="AE3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH3" s="6">
         <v>44208</v>
       </c>
-      <c r="N3" s="5">
+      <c r="AI3" s="5">
         <v>13500000</v>
       </c>
-      <c r="O3" s="8">
+      <c r="AJ3" s="8">
         <v>44050</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2">
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2">
         <v>0.9</v>
       </c>
-      <c r="H4">
+      <c r="N4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="R4" t="s">
         <v>87</v>
       </c>
-      <c r="J4" t="s">
+      <c r="S4" t="s">
+        <v>87</v>
+      </c>
+      <c r="T4" t="s">
+        <v>133</v>
+      </c>
+      <c r="U4" t="s">
+        <v>136</v>
+      </c>
+      <c r="V4" t="s">
         <v>81</v>
       </c>
-      <c r="K4" t="s">
+      <c r="W4" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z4" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
+      <c r="AA4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD4" t="s">
         <v>32</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AE4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH4" t="s">
         <v>81</v>
       </c>
-      <c r="N4" s="5">
+      <c r="AI4" s="5">
         <v>5300000</v>
       </c>
-      <c r="O4" s="8">
+      <c r="AJ4" s="8">
         <v>44120</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -974,40 +1391,103 @@
       <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="L5" s="3"/>
       <c r="M5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" t="s">
+        <v>142</v>
+      </c>
+      <c r="P5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" t="s">
+        <v>81</v>
+      </c>
+      <c r="X5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI5" s="5">
         <v>0</v>
       </c>
-      <c r="O5" s="5"/>
+      <c r="AJ5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1017,44 +1497,103 @@
       <c r="C6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" t="s">
         <v>80</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
-        <v>32</v>
       </c>
       <c r="M6" t="s">
         <v>81</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" t="s">
+        <v>142</v>
+      </c>
+      <c r="P6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" t="s">
+        <v>81</v>
+      </c>
+      <c r="W6" t="s">
+        <v>81</v>
+      </c>
+      <c r="X6" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI6" s="5">
         <v>5000000</v>
       </c>
-      <c r="O6" s="8">
+      <c r="AJ6" s="8">
         <v>44230</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1064,46 +1603,117 @@
       <c r="C7" t="s">
         <v>84</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
         <v>85</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>86</v>
       </c>
-      <c r="G7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="M7" t="s">
         <v>81</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" t="s">
+        <v>81</v>
+      </c>
+      <c r="W7" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI7" s="5">
         <v>6000000</v>
       </c>
-      <c r="O7" s="8">
+      <c r="AJ7" s="8">
         <v>44230</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{AA5AA6B6-ABB5-48C2-9260-9D4AA70505D2}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{D8E7C985-1C29-4446-8763-A13A8F01DBCC}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{35B95353-90B9-494D-B57E-686C12ECFE8C}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{9FD06C4C-3718-482D-B668-BC41187588C1}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{B4470BCD-342F-47EC-99C6-D91C0364A4B6}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{9E54B9FC-3A4D-45B8-8717-669DEA76444E}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{D8BA6122-D061-4A72-A474-2C53C0A8DFBB}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{9B4094D8-0DAF-4B5B-A97F-8353A2D0886A}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{4EC2CAB3-89EB-4EC6-B3E8-E214D5FE0DB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1111,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1350,6 +1960,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -1527,15 +2146,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
@@ -1546,6 +2156,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1561,12 +2179,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
i18n hotfix vaccines information
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6000A9F2-BF7D-4841-B001-EF750617AAD3}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6DBBEC7-73A8-417A-966E-9434F591AF6F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="165">
   <si>
     <t>manufacturer</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>effectiveness_fr</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Tozinameran</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Tozinam%C3%A9ran</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -613,6 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -931,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -944,7 +951,10 @@
     <col min="9" max="11" width="47.21875" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
     <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="29" width="14.77734375" customWidth="1"/>
+    <col min="18" max="19" width="14.77734375" customWidth="1"/>
+    <col min="20" max="20" width="21.109375" customWidth="1"/>
+    <col min="21" max="21" width="23.5546875" customWidth="1"/>
+    <col min="22" max="29" width="14.77734375" customWidth="1"/>
     <col min="30" max="30" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="8.44140625" customWidth="1"/>
     <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -1010,10 +1020,10 @@
         <v>128</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>26</v>
@@ -1068,14 +1078,18 @@
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="G2" t="s">
         <v>22</v>
       </c>
@@ -1497,11 +1511,15 @@
       <c r="C6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="E6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="G6" t="s">
         <v>80</v>
       </c>
@@ -1711,9 +1729,12 @@
     <hyperlink ref="D3" r:id="rId7" xr:uid="{D8BA6122-D061-4A72-A474-2C53C0A8DFBB}"/>
     <hyperlink ref="E3" r:id="rId8" xr:uid="{9B4094D8-0DAF-4B5B-A97F-8353A2D0886A}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{4EC2CAB3-89EB-4EC6-B3E8-E214D5FE0DB3}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{615A83B7-9CA4-4ECB-A815-C5FF26B70131}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{4DEEC3C2-1E33-457C-9E5E-9D668888C402}"/>
+    <hyperlink ref="C2" r:id="rId12" xr:uid="{0D5EBA99-7ED1-4E36-B64F-62967A98CE76}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1960,15 +1981,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -2146,6 +2158,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
@@ -2156,14 +2177,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2179,4 +2192,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
i18n titles in vaccines information
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6DBBEC7-73A8-417A-966E-9434F591AF6F}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47A541A7-2D69-4FA3-9306-A01FA129FFA8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="9900" yWindow="0" windowWidth="24324" windowHeight="8304" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="170">
   <si>
     <t>manufacturer</t>
   </si>
@@ -195,24 +195,9 @@
     <t>Next-generation vaccine platforms for COVID-19</t>
   </si>
   <si>
-    <t>SRF:</t>
-  </si>
-  <si>
-    <t>Admin.ch:</t>
-  </si>
-  <si>
-    <t>swissmedic:</t>
-  </si>
-  <si>
     <t>how and why do vaccines act in the body.</t>
   </si>
   <si>
-    <t>swissinfo.ch:</t>
-  </si>
-  <si>
-    <t>nature comment:</t>
-  </si>
-  <si>
     <t>cooling temperature</t>
   </si>
   <si>
@@ -225,9 +210,6 @@
     <t>COVID-19 Vaccine AstraZeneca</t>
   </si>
   <si>
-    <t>Bundesamt für Statistik (BAG)</t>
-  </si>
-  <si>
     <t>details_en</t>
   </si>
   <si>
@@ -255,9 +237,6 @@
     <t>Next-generation vaccine platforms for COVID-19 (english)</t>
   </si>
   <si>
-    <t xml:space="preserve">Wikipedia: </t>
-  </si>
-  <si>
     <t>COVID-19 vaccine</t>
   </si>
   <si>
@@ -529,6 +508,42 @@
   </si>
   <si>
     <t>https://fr.wikipedia.org/wiki/Tozinam%C3%A9ran</t>
+  </si>
+  <si>
+    <t>title_en</t>
+  </si>
+  <si>
+    <t>title_de</t>
+  </si>
+  <si>
+    <t>title_fr</t>
+  </si>
+  <si>
+    <t>Bundesamt für Gesundheit (BAG)</t>
+  </si>
+  <si>
+    <t>Office fédéral de la santé publique (OFSP)</t>
+  </si>
+  <si>
+    <t>Federal Office of Public Health (FOPH)</t>
+  </si>
+  <si>
+    <t>SRF</t>
+  </si>
+  <si>
+    <t>Admin.ch</t>
+  </si>
+  <si>
+    <t>swissmedic</t>
+  </si>
+  <si>
+    <t>swissinfo.ch</t>
+  </si>
+  <si>
+    <t>nature comment</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
   </si>
 </sst>
 </file>
@@ -938,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -972,13 +987,13 @@
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>21</v>
@@ -987,13 +1002,13 @@
         <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -1002,13 +1017,13 @@
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>2</v>
@@ -1017,49 +1032,49 @@
         <v>39</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="AD1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>15</v>
@@ -1085,10 +1100,10 @@
         <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
@@ -1100,10 +1115,10 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>14</v>
@@ -1124,16 +1139,16 @@
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="T2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="U2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="V2" t="s">
         <v>25</v>
@@ -1142,10 +1157,10 @@
         <v>25</v>
       </c>
       <c r="X2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="Y2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>41</v>
@@ -1164,10 +1179,10 @@
         <v>7</v>
       </c>
       <c r="AF2" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="AG2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="AH2" s="6">
         <v>44184</v>
@@ -1193,10 +1208,10 @@
         <v>47</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
@@ -1208,10 +1223,10 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>14</v>
@@ -1232,16 +1247,16 @@
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="T3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="U3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="V3" t="s">
         <v>29</v>
@@ -1250,10 +1265,10 @@
         <v>29</v>
       </c>
       <c r="X3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="Y3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="Z3" s="10" t="s">
         <v>42</v>
@@ -1272,10 +1287,10 @@
         <v>7</v>
       </c>
       <c r="AF3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="AG3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="AH3" s="6">
         <v>44208</v>
@@ -1292,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>46</v>
@@ -1301,10 +1316,10 @@
         <v>46</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
@@ -1316,10 +1331,10 @@
         <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="K4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="2">
@@ -1338,28 +1353,28 @@
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="S4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="T4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="U4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="V4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="W4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="X4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Y4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Z4" t="s">
         <v>40</v>
@@ -1368,10 +1383,10 @@
         <v>40</v>
       </c>
       <c r="AB4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="AC4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AD4" t="s">
         <v>32</v>
@@ -1380,13 +1395,13 @@
         <v>32</v>
       </c>
       <c r="AF4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="AG4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AH4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AI4" s="5">
         <v>5300000</v>
@@ -1409,10 +1424,10 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -1424,23 +1439,23 @@
         <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="O5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -1458,16 +1473,16 @@
         <v>13</v>
       </c>
       <c r="V5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="W5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="X5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Y5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Z5" t="s">
         <v>31</v>
@@ -1476,10 +1491,10 @@
         <v>31</v>
       </c>
       <c r="AB5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="AC5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="AD5" t="s">
         <v>32</v>
@@ -1488,13 +1503,13 @@
         <v>32</v>
       </c>
       <c r="AF5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="AG5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AH5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AI5" s="5">
         <v>0</v>
@@ -1503,25 +1518,25 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -1530,25 +1545,25 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L6" t="s">
         <v>14</v>
       </c>
       <c r="M6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="O6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P6" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Q6">
         <v>2</v>
@@ -1566,16 +1581,16 @@
         <v>13</v>
       </c>
       <c r="V6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="W6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="X6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Y6" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Z6" t="s">
         <v>31</v>
@@ -1584,10 +1599,10 @@
         <v>31</v>
       </c>
       <c r="AB6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="AC6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="AD6" t="s">
         <v>32</v>
@@ -1596,13 +1611,13 @@
         <v>32</v>
       </c>
       <c r="AF6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="AG6" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AH6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AI6" s="5">
         <v>5000000</v>
@@ -1613,49 +1628,49 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="K7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="M7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="O7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Q7">
         <v>2</v>
@@ -1673,16 +1688,16 @@
         <v>13</v>
       </c>
       <c r="V7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="W7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="X7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Y7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="Z7" t="s">
         <v>40</v>
@@ -1691,10 +1706,10 @@
         <v>40</v>
       </c>
       <c r="AB7" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="AC7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="AD7" t="s">
         <v>32</v>
@@ -1703,13 +1718,13 @@
         <v>32</v>
       </c>
       <c r="AF7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="AG7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AH7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AI7" s="5">
         <v>6000000</v>
@@ -1740,234 +1755,307 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="68.21875" customWidth="1"/>
-    <col min="5" max="5" width="117.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="68.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="68.21875" customWidth="1"/>
+    <col min="8" max="8" width="117.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>94</v>
+      <c r="I1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>105</v>
+      <c r="K2" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
       </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>101</v>
+      <c r="K4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
         <v>90</v>
       </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>98</v>
+      <c r="K5" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
       </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
         <v>51</v>
       </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>76</v>
+        <v>169</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H8" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{C67C19B8-C4B8-4EC7-9BB4-19ED833F6A9E}"/>
-    <hyperlink ref="F8" r:id="rId3" xr:uid="{DE30262E-6002-4DA8-B4D5-4CDF00B10510}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{382C03B7-1942-4F53-8F24-A40AC7CC5598}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{C67C19B8-C4B8-4EC7-9BB4-19ED833F6A9E}"/>
+    <hyperlink ref="I8" r:id="rId3" xr:uid="{DE30262E-6002-4DA8-B4D5-4CDF00B10510}"/>
+    <hyperlink ref="J2" r:id="rId4" xr:uid="{382C03B7-1942-4F53-8F24-A40AC7CC5598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>

</xml_diff>

<commit_message>
pfizer up to 6M (now correct file)
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47A541A7-2D69-4FA3-9306-A01FA129FFA8}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{819070E4-755C-4BA2-9B84-DCB7E82C9F3B}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="0" windowWidth="24324" windowHeight="8304" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="10020" yWindow="1896" windowWidth="19992" windowHeight="13992" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1188,7 @@
         <v>44184</v>
       </c>
       <c r="AI2" s="5">
-        <v>3000000</v>
+        <v>6000000</v>
       </c>
       <c r="AJ2" s="8">
         <v>44172</v>
@@ -1757,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2069,6 +2069,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -2246,15 +2255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
@@ -2265,6 +2265,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2280,12 +2288,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to approval of Jansen and order volumes
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{819070E4-755C-4BA2-9B84-DCB7E82C9F3B}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23843155-CDBE-43E4-A783-D01C48980B9B}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="1896" windowWidth="19992" windowHeight="13992" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="18840" yWindow="6348" windowWidth="23040" windowHeight="12204" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="174">
   <si>
     <t>manufacturer</t>
   </si>
@@ -69,9 +69,6 @@
     <t>reserved doses</t>
   </si>
   <si>
-    <t>Janssen-Cilag</t>
-  </si>
-  <si>
     <t>DE (part of Johnson &amp; Johnson (US))</t>
   </si>
   <si>
@@ -544,6 +541,21 @@
   </si>
   <si>
     <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Johnson &amp; Johnson / Janssen-Cilag</t>
+  </si>
+  <si>
+    <t>https://www.swissmedic.ch/swissmedic/en/home/news/coronavirus-covid-19/dritten-impfstoff-gegen-covid-19-erkrankung.html</t>
+  </si>
+  <si>
+    <t>Zulassungsverfahren abgebrochen</t>
+  </si>
+  <si>
+    <t>approval process aborted</t>
+  </si>
+  <si>
+    <t>procédure d'approbation interrompue</t>
   </si>
 </sst>
 </file>
@@ -581,7 +593,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,6 +618,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -621,7 +639,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -631,10 +649,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -951,10 +974,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -981,34 +1007,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -1017,288 +1043,292 @@
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="AD1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AE1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="AG1" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="AH1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="N2" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P2" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>2</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="W2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="Q2">
+      <c r="X2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH2" s="14">
+        <v>44184</v>
+      </c>
+      <c r="AI2" s="15">
+        <v>20000000</v>
+      </c>
+      <c r="AJ2" s="16">
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="N3" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="O3" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="P3" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="Q3" s="10">
         <v>2</v>
       </c>
-      <c r="R2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" t="s">
-        <v>56</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="R3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="V2" t="s">
-        <v>25</v>
-      </c>
-      <c r="W2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="V3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AA3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" t="s">
+      <c r="AC3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>44184</v>
-      </c>
-      <c r="AI2" s="5">
-        <v>6000000</v>
-      </c>
-      <c r="AJ2" s="8">
-        <v>44172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" t="s">
-        <v>125</v>
-      </c>
-      <c r="U3" t="s">
-        <v>128</v>
-      </c>
-      <c r="V3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" t="s">
-        <v>29</v>
-      </c>
-      <c r="X3" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC3" s="10"/>
-      <c r="AD3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AH3" s="6">
+      <c r="AF3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH3" s="14">
         <v>44208</v>
       </c>
-      <c r="AI3" s="5">
-        <v>13500000</v>
-      </c>
-      <c r="AJ3" s="8">
+      <c r="AI3" s="15">
+        <v>20500000</v>
+      </c>
+      <c r="AJ3" s="16">
         <v>44050</v>
       </c>
     </row>
@@ -1307,34 +1337,34 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>106</v>
+        <v>56</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="2">
@@ -1353,55 +1383,55 @@
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC4" t="s">
         <v>142</v>
       </c>
-      <c r="AC4" t="s">
-        <v>143</v>
-      </c>
       <c r="AD4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE4" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="AF4" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="AG4" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="AH4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI4" s="5">
         <v>5300000</v>
@@ -1410,214 +1440,216 @@
         <v>44120</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G5" t="s">
+      <c r="L5" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="M5" s="17">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="P5" s="17">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>1</v>
+      </c>
+      <c r="R5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K5" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" t="s">
-        <v>135</v>
-      </c>
-      <c r="P5" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U5" t="s">
-        <v>13</v>
-      </c>
-      <c r="V5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W5" t="s">
-        <v>74</v>
-      </c>
-      <c r="X5" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>150</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="S5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="AH5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="5"/>
+      <c r="AH5" s="14">
+        <v>44277</v>
+      </c>
+      <c r="AI5" s="15">
+        <v>150000</v>
+      </c>
+      <c r="AJ5" s="15"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K6" t="s">
-        <v>114</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" t="s">
-        <v>74</v>
-      </c>
       <c r="N6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q6">
         <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD6" t="s">
         <v>31</v>
       </c>
-      <c r="AA6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>32</v>
-      </c>
       <c r="AE6" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="AF6" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="AG6" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="AH6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI6" s="5">
         <v>5000000</v>
@@ -1628,103 +1660,103 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>112</v>
       </c>
-      <c r="G7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" t="s">
-        <v>113</v>
-      </c>
       <c r="M7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q7">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC7" t="s">
         <v>142</v>
       </c>
-      <c r="AC7" t="s">
-        <v>143</v>
-      </c>
       <c r="AD7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AF7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG7" t="s">
         <v>150</v>
       </c>
-      <c r="AG7" t="s">
-        <v>151</v>
-      </c>
       <c r="AH7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI7" s="5">
         <v>6000000</v>
@@ -1732,6 +1764,10 @@
       <c r="AJ7" s="8">
         <v>44230</v>
       </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AF8" s="7"/>
+      <c r="AH8" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1772,95 +1808,95 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="I1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
         <v>161</v>
       </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" t="s">
-        <v>162</v>
-      </c>
       <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
       <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>16</v>
+        <v>81</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -1877,177 +1913,177 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
         <v>93</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
         <v>90</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>69</v>
+      <c r="I8" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2063,21 +2099,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -2255,24 +2276,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2288,4 +2307,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed not approved / approved
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23843155-CDBE-43E4-A783-D01C48980B9B}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E58439D-D8E5-48A7-9E0B-40A02DE7BBF9}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="6348" windowWidth="23040" windowHeight="12204" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="175">
   <si>
     <t>manufacturer</t>
   </si>
@@ -549,13 +549,16 @@
     <t>https://www.swissmedic.ch/swissmedic/en/home/news/coronavirus-covid-19/dritten-impfstoff-gegen-covid-19-erkrankung.html</t>
   </si>
   <si>
-    <t>Zulassungsverfahren abgebrochen</t>
-  </si>
-  <si>
-    <t>approval process aborted</t>
-  </si>
-  <si>
-    <t>procédure d'approbation interrompue</t>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Mittelwert</t>
+  </si>
+  <si>
+    <t>Laufende Summe</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
   </si>
 </sst>
 </file>
@@ -977,10 +980,10 @@
   <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE11" sqref="AE11"/>
+      <selection pane="bottomRight" activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -997,7 +1000,9 @@
     <col min="21" max="21" width="23.5546875" customWidth="1"/>
     <col min="22" max="29" width="14.77734375" customWidth="1"/>
     <col min="30" max="30" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="8.44140625" customWidth="1"/>
+    <col min="31" max="31" width="22" customWidth="1"/>
+    <col min="32" max="32" width="26.77734375" customWidth="1"/>
+    <col min="33" max="33" width="8.44140625" customWidth="1"/>
     <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="17.44140625" customWidth="1"/>
   </cols>
@@ -1422,13 +1427,13 @@
         <v>31</v>
       </c>
       <c r="AE4" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
       <c r="AF4" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="AG4" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="AH4" t="s">
         <v>73</v>
@@ -1640,13 +1645,13 @@
         <v>31</v>
       </c>
       <c r="AE6" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
       <c r="AF6" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="AG6" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="AH6" t="s">
         <v>73</v>
@@ -2099,6 +2104,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -2276,22 +2296,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2307,21 +2329,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
vaccine states: only two different states
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awkgroup-my.sharepoint.com/personal/waj_awk_ch/Documents/80_prog/projects/petproject_impfcounter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="295" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65B575BC-6899-4A3E-8C81-D5F9D12541E3}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{076AEACA-8775-4E9B-A1B1-72BD6CBA883B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC58CB28-7AD9-4BDD-9E72-9F2C9C31D2AD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="-5240" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="169">
   <si>
     <t>manufacturer</t>
   </si>
@@ -481,12 +481,6 @@
   </si>
   <si>
     <t>zugelassen</t>
-  </si>
-  <si>
-    <t>im Zulassungsverfahren</t>
-  </si>
-  <si>
-    <t>en cours de procédure d'approbation</t>
   </si>
   <si>
     <t>autorisé</t>
@@ -971,7 +965,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH18" sqref="AH18"/>
+      <selection pane="bottomRight" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -987,10 +981,10 @@
     <col min="20" max="20" width="21.109375" customWidth="1"/>
     <col min="21" max="21" width="23.5546875" customWidth="1"/>
     <col min="22" max="29" width="14.77734375" customWidth="1"/>
-    <col min="30" max="30" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22" customWidth="1"/>
+    <col min="30" max="30" width="20.109375" customWidth="1"/>
+    <col min="31" max="31" width="27.21875" customWidth="1"/>
     <col min="32" max="32" width="26.77734375" customWidth="1"/>
-    <col min="33" max="33" width="8.44140625" customWidth="1"/>
+    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="17.44140625" customWidth="1"/>
   </cols>
@@ -1036,13 +1030,13 @@
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>2</v>
@@ -1119,10 +1113,10 @@
         <v>47</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>21</v>
@@ -1203,7 +1197,7 @@
         <v>148</v>
       </c>
       <c r="AG2" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AH2" s="14">
         <v>44184</v>
@@ -1313,7 +1307,7 @@
         <v>148</v>
       </c>
       <c r="AG3" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AH3" s="14">
         <v>44208</v>
@@ -1327,7 +1321,7 @@
     </row>
     <row r="4" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>32</v>
@@ -1360,7 +1354,7 @@
         <v>115</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M4" s="17">
         <v>0.66900000000000004</v>
@@ -1423,7 +1417,7 @@
         <v>148</v>
       </c>
       <c r="AG4" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AH4" s="14">
         <v>44277</v>
@@ -1740,13 +1734,13 @@
         <v>31</v>
       </c>
       <c r="AE7" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="AF7" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="AG7" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="AH7" t="s">
         <v>73</v>
@@ -1804,13 +1798,13 @@
         <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>57</v>
@@ -1836,16 +1830,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
         <v>160</v>
       </c>
-      <c r="B2" t="s">
-        <v>162</v>
-      </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -1871,16 +1865,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
         <v>95</v>
@@ -1906,16 +1900,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -1941,16 +1935,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
         <v>52</v>
@@ -1976,16 +1970,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -2011,16 +2005,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
         <v>51</v>
@@ -2046,16 +2040,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
         <v>66</v>
@@ -2098,6 +2092,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -2275,15 +2278,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
   <ds:schemaRefs>
@@ -2294,6 +2288,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2309,12 +2311,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>